<commit_message>
[Feat] 유물 UI 작업 중
</commit_message>
<xml_diff>
--- a/Assets/Excel/ArtifactSO.xlsx
+++ b/Assets/Excel/ArtifactSO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whals\OneDrive\Desktop\workspace\TeamProject_CheerUpMyHero\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B694FDEC-BE93-4742-A982-98CE72A9192F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D795852-928C-483D-AE7C-3109E59F77BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9490" yWindow="3410" windowWidth="17700" windowHeight="12670" activeTab="1" xr2:uid="{2DCCF674-CAD7-453F-824C-C429D706D6A1}"/>
+    <workbookView xWindow="2970" yWindow="730" windowWidth="22930" windowHeight="15410" activeTab="1" xr2:uid="{2DCCF674-CAD7-453F-824C-C429D706D6A1}"/>
   </bookViews>
   <sheets>
     <sheet name="activeArtifacts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="101">
   <si>
     <t>idNumber</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,21 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>commonValue</t>
-  </si>
-  <si>
-    <t>rareValue</t>
-  </si>
-  <si>
-    <t>epicValue</t>
-  </si>
-  <si>
-    <t>uniqueValue</t>
-  </si>
-  <si>
-    <t>legendaryValue</t>
-  </si>
-  <si>
     <t>level</t>
   </si>
   <si>
@@ -198,30 +183,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>플레이어의 공격력을 %로 증가</t>
-  </si>
-  <si>
-    <t>플레이어의 체력을 %로 증가</t>
-  </si>
-  <si>
-    <t>플레이어의 이동 속도를 %로 증가</t>
-  </si>
-  <si>
-    <t>플레이어의 오라 범위를 %로 증가</t>
-  </si>
-  <si>
-    <t>모든 근거리 유닛의 공격력을 %로 증가</t>
-  </si>
-  <si>
-    <t>모든 근거리 유닛의 체력을 %로 증가</t>
-  </si>
-  <si>
-    <t>모든 원거리 유닛의 공격력을 %로 증가</t>
-  </si>
-  <si>
-    <t>모든 원거리 유닛의 체력을 %로 증가</t>
-  </si>
-  <si>
     <t>Passive</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -235,28 +196,180 @@
     <t>RangedUnit</t>
   </si>
   <si>
-    <t>PlayerAttackPower</t>
-  </si>
-  <si>
-    <t>PlayerHealth</t>
-  </si>
-  <si>
-    <t>PlayerMoveSpeed</t>
-  </si>
-  <si>
-    <t>PlayerAuraRange</t>
-  </si>
-  <si>
-    <t>MeleeUnitAttackPower</t>
-  </si>
-  <si>
-    <t>MeleeUnitHealth</t>
-  </si>
-  <si>
-    <t>RangedUnitAttackPower</t>
-  </si>
-  <si>
-    <t>RangedUnitHealth</t>
+    <t>grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>AtkPower</t>
+  </si>
+  <si>
+    <t>MaxHp</t>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+  </si>
+  <si>
+    <t>AuraRange</t>
+  </si>
+  <si>
+    <t>플레이어의 공격력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 공격력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 공격력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 공격력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 공격력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 체력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 체력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 체력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 체력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 체력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 이동 속도를 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 이동 속도를 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 이동 속도를 15%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 이동 속도를 20%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 이동 속도를 25%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 오라 범위를 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 오라 범위를 20%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 오라 범위를 30%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 오라 범위를 40%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어의 오라 범위를 50%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 공격력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 공격력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 공격력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 공격력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 공격력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 체력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 체력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 체력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 체력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>모든 근거리 유닛의 체력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 공격력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 공격력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 공격력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 공격력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 공격력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 체력을 5%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 체력을 10%로 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 체력을 15%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 체력을 20%로 증가</t>
+  </si>
+  <si>
+    <t>모든 원거리 유닛의 체력을 25%로 증가</t>
+  </si>
+  <si>
+    <t>플레이어 전방 범위의 적들에게 (피해량%)의 광역 피해를 주고, 15초 동안 이동 속도와 공격 속도를 15% 감소 시킵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -639,7 +752,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -682,16 +795,16 @@
         <v>8010001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="F2" s="2">
         <v>3</v>
@@ -702,16 +815,16 @@
         <v>8010002</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
@@ -722,16 +835,16 @@
         <v>8010003</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
@@ -742,16 +855,16 @@
         <v>8010004</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2">
         <v>10</v>
@@ -762,16 +875,16 @@
         <v>8010005</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2">
         <v>15</v>
@@ -795,10 +908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169A894D-86E5-49E7-834E-05CA49D6DD71}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -809,14 +922,15 @@
     <col min="4" max="4" width="10.9140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,304 +950,1111 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>8020001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="2">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="2">
         <v>5</v>
       </c>
-      <c r="H2" s="2">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>8020001</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>8020002</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="2">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
       </c>
       <c r="H3" s="2">
         <v>10</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>8020001</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2">
         <v>15</v>
       </c>
-      <c r="J3" s="2">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>8020001</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>8020003</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="2">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2">
-        <v>15</v>
-      </c>
-      <c r="J4" s="2">
-        <v>20</v>
-      </c>
-      <c r="K4" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>8020004</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="2">
-        <v>10</v>
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
       </c>
       <c r="H5" s="2">
         <v>20</v>
       </c>
-      <c r="I5" s="2">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2">
-        <v>40</v>
-      </c>
-      <c r="K5" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>8020005</v>
+        <v>8020001</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="2">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>8020002</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>8020002</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2">
-        <v>15</v>
-      </c>
-      <c r="J6" s="2">
-        <v>20</v>
-      </c>
-      <c r="K6" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>8020006</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>10</v>
-      </c>
-      <c r="I7" s="2">
-        <v>15</v>
-      </c>
-      <c r="J7" s="2">
-        <v>20</v>
-      </c>
-      <c r="K7" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>8020007</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
       </c>
       <c r="H8" s="2">
         <v>10</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8020002</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="2">
         <v>15</v>
       </c>
-      <c r="J8" s="2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>8020002</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="2">
         <v>20</v>
       </c>
-      <c r="K8" s="2">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>8020002</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>8020003</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>8020003</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>8020003</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>8020003</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>8020003</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>8020004</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>8020004</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>8020004</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>8020004</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>8020004</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>8020005</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>8020005</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>8020005</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>8020005</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>8020005</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>8020006</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>8020006</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>8020006</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>8020006</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>8020006</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>8020007</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>8020007</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>8020007</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>8020007</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>8020007</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
         <v>8020008</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="2">
         <v>5</v>
       </c>
-      <c r="H9" s="2">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>8020008</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="2">
         <v>10</v>
       </c>
-      <c r="I9" s="2">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>8020008</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="2">
         <v>15</v>
       </c>
-      <c r="J9" s="2">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>8020008</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="2">
         <v>20</v>
       </c>
-      <c r="K9" s="2">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>8020008</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="2">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1143,7 +2064,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1177,40 +2098,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.45">
@@ -1218,13 +2139,13 @@
         <v>8010001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1250,13 +2171,13 @@
         <v>8010001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1282,13 +2203,13 @@
         <v>8010001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1317,13 +2238,13 @@
         <v>8010001</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1352,13 +2273,13 @@
         <v>8010001</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1387,13 +2308,13 @@
         <v>8010001</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1422,13 +2343,13 @@
         <v>8010001</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1457,13 +2378,13 @@
         <v>8010001</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1492,13 +2413,13 @@
         <v>8010001</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -1527,13 +2448,13 @@
         <v>8010002</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1559,13 +2480,13 @@
         <v>8010002</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1591,13 +2512,13 @@
         <v>8010002</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1626,13 +2547,13 @@
         <v>8010002</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1661,13 +2582,13 @@
         <v>8010002</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1696,13 +2617,13 @@
         <v>8010002</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -1731,13 +2652,13 @@
         <v>8010002</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>7</v>
@@ -1766,13 +2687,13 @@
         <v>8010002</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E18">
         <v>8</v>
@@ -1801,13 +2722,13 @@
         <v>8010002</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>9</v>
@@ -1836,13 +2757,13 @@
         <v>8010003</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1871,13 +2792,13 @@
         <v>8010003</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1906,13 +2827,13 @@
         <v>8010003</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -1944,13 +2865,13 @@
         <v>8010003</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -1982,13 +2903,13 @@
         <v>8010003</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E24">
         <v>5</v>
@@ -2020,13 +2941,13 @@
         <v>8010003</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E25">
         <v>6</v>
@@ -2058,13 +2979,13 @@
         <v>8010003</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E26">
         <v>7</v>
@@ -2096,13 +3017,13 @@
         <v>8010003</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>8</v>
@@ -2134,13 +3055,13 @@
         <v>8010003</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E28">
         <v>9</v>
@@ -2172,13 +3093,13 @@
         <v>8010004</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2204,13 +3125,13 @@
         <v>8010004</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2236,13 +3157,13 @@
         <v>8010004</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -2271,13 +3192,13 @@
         <v>8010004</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -2306,13 +3227,13 @@
         <v>8010004</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -2341,13 +3262,13 @@
         <v>8010004</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E34">
         <v>6</v>
@@ -2376,13 +3297,13 @@
         <v>8010004</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E35">
         <v>7</v>
@@ -2411,13 +3332,13 @@
         <v>8010004</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E36">
         <v>8</v>
@@ -2446,13 +3367,13 @@
         <v>8010004</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E37">
         <v>9</v>
@@ -2481,13 +3402,13 @@
         <v>8010005</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2516,13 +3437,13 @@
         <v>8010005</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -2551,13 +3472,13 @@
         <v>8010005</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -2589,13 +3510,13 @@
         <v>8010005</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2627,13 +3548,13 @@
         <v>8010005</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -2665,13 +3586,13 @@
         <v>8010005</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -2703,13 +3624,13 @@
         <v>8010005</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E44">
         <v>7</v>
@@ -2741,13 +3662,13 @@
         <v>8010005</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E45">
         <v>8</v>
@@ -2779,13 +3700,13 @@
         <v>8010005</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E46">
         <v>9</v>

</xml_diff>